<commit_message>
major changes. completed main task. alsoa added more folders. created a tr_script that is synchronized only to tr. From now on, only minor changes.
</commit_message>
<xml_diff>
--- a/events/sub-test_task-sentences_events.xlsx
+++ b/events/sub-test_task-sentences_events.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="52" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="679" uniqueCount="8">
   <si>
     <t>TR</t>
   </si>
@@ -31,6 +31,12 @@
   </si>
   <si>
     <t>Active Stimuli</t>
+  </si>
+  <si>
+    <t>Cross</t>
+  </si>
+  <si>
+    <t>Neutral Stimuli</t>
   </si>
 </sst>
 </file>
@@ -82,11 +88,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="3.28515625" customWidth="true"/>
-    <col min="2" max="2" width="13.5703125" customWidth="true"/>
-    <col min="3" max="3" width="12.85546875" customWidth="true"/>
-    <col min="4" max="4" width="11.7109375" customWidth="true"/>
-    <col min="5" max="5" width="13.42578125" customWidth="true"/>
+    <col min="1" max="1" width="3.109375" customWidth="true"/>
+    <col min="2" max="2" width="12.109375" customWidth="true"/>
+    <col min="3" max="3" width="11.5546875" customWidth="true"/>
+    <col min="4" max="4" width="11.5546875" customWidth="true"/>
+    <col min="5" max="5" width="11.88671875" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -111,13 +117,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>1.9967132000019774</v>
+        <v>1.9998282999986259</v>
       </c>
       <c r="C2" s="0">
-        <v>934480.68609500001</v>
+        <v>22520.735716199997</v>
       </c>
       <c r="D2" s="0">
-        <v>934484.68988720002</v>
+        <v>22524.737346099999</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>5</v>
@@ -128,13 +134,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>3.9964576000347733</v>
+        <v>3.9993566000011924</v>
       </c>
       <c r="C3" s="0">
-        <v>934480.686154</v>
+        <v>22520.7359922</v>
       </c>
       <c r="D3" s="0">
-        <v>934486.68963160005</v>
+        <v>22526.736874400001</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>5</v>
@@ -145,13 +151,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>5.9953248000238091</v>
+        <v>5.9990049000007275</v>
       </c>
       <c r="C4" s="0">
-        <v>934480.68660510005</v>
+        <v>22520.7361217</v>
       </c>
       <c r="D4" s="0">
-        <v>934488.68849880004</v>
+        <v>22528.736522700001</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>5</v>
@@ -162,13 +168,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>7.9957216000184417</v>
+        <v>7.9992920000004233</v>
       </c>
       <c r="C5" s="0">
-        <v>934480.68660630006</v>
+        <v>22520.736121599999</v>
       </c>
       <c r="D5" s="0">
-        <v>934490.68889560003</v>
+        <v>22530.736809800001</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>5</v>
@@ -176,190 +182,168 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B6" s="0">
-        <v>9.9952970999293029</v>
+        <v>0</v>
       </c>
       <c r="C6" s="0">
-        <v>934480.68660529994</v>
+        <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>934492.68847109994</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E6" s="0"/>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B7" s="0">
-        <v>11.99499040003866</v>
+        <v>0</v>
       </c>
       <c r="C7" s="0">
-        <v>934480.68660260004</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>934494.68816440005</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E7" s="0"/>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B8" s="0">
-        <v>13.995282799936831</v>
+        <v>0</v>
       </c>
       <c r="C8" s="0">
-        <v>934480.68660259992</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>934496.68845679995</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E8" s="0"/>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B9" s="0">
-        <v>15.995782800018787</v>
+        <v>0</v>
       </c>
       <c r="C9" s="0">
-        <v>934480.68659110006</v>
+        <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>934498.68895680003</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E9" s="0"/>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B10" s="0">
-        <v>17.997794199967757</v>
+        <v>0</v>
       </c>
       <c r="C10" s="0">
-        <v>934480.68660270004</v>
+        <v>0</v>
       </c>
       <c r="D10" s="0">
-        <v>934500.69096819998</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E10" s="0"/>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="B11" s="0">
-        <v>19.995780400000513</v>
+        <v>0</v>
       </c>
       <c r="C11" s="0">
-        <v>934480.68660580006</v>
+        <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>934502.68895440002</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E11" s="0"/>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B12" s="0">
-        <v>21.99546130001545</v>
+        <v>0</v>
       </c>
       <c r="C12" s="0">
-        <v>934480.68660380004</v>
+        <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>934504.68863530003</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E12" s="0"/>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B13" s="0">
-        <v>23.994809999945574</v>
+        <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>934480.68660629995</v>
+        <v>0</v>
       </c>
       <c r="D13" s="0">
-        <v>934506.68798399996</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E13" s="0"/>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B14" s="0">
-        <v>25.996047999942675</v>
+        <v>0</v>
       </c>
       <c r="C14" s="0">
-        <v>934480.68660379993</v>
+        <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>934508.68922199996</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E14" s="0"/>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B15" s="0">
-        <v>27.995392399956472</v>
+        <v>0</v>
       </c>
       <c r="C15" s="0">
-        <v>934480.68660319992</v>
+        <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>934510.68856639997</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E15" s="0"/>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B16" s="0">
-        <v>29.996707499958575</v>
+        <v>0</v>
       </c>
       <c r="C16" s="0">
-        <v>934480.68659199995</v>
+        <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>934512.68988149997</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>5</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="E16" s="0"/>
     </row>
     <row r="17">
       <c r="A17" s="0">

</xml_diff>

<commit_message>
feature: fixed event output and added event files from participants
</commit_message>
<xml_diff>
--- a/events/sub-test_task-sentences_events.xlsx
+++ b/events/sub-test_task-sentences_events.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="679" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1798" uniqueCount="8">
   <si>
     <t>TR</t>
   </si>
@@ -117,13 +117,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>1.9998282999986259</v>
+        <v>1.9997048999648541</v>
       </c>
       <c r="C2" s="0">
-        <v>22520.735716199997</v>
+        <v>2018076.0184128999</v>
       </c>
       <c r="D2" s="0">
-        <v>22524.737346099999</v>
+        <v>2018078.0202494999</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>5</v>
@@ -134,13 +134,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>3.9993566000011924</v>
+        <v>3.9987212000414729</v>
       </c>
       <c r="C3" s="0">
-        <v>22520.7359922</v>
+        <v>2018076.0185197999</v>
       </c>
       <c r="D3" s="0">
-        <v>22526.736874400001</v>
+        <v>2018080.0192658</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>5</v>
@@ -151,13 +151,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>5.9990049000007275</v>
+        <v>5.998412000015378</v>
       </c>
       <c r="C4" s="0">
-        <v>22520.7361217</v>
+        <v>2018076.0186335</v>
       </c>
       <c r="D4" s="0">
-        <v>22528.736522700001</v>
+        <v>2018082.0189566</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>5</v>
@@ -168,13 +168,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>7.9992920000004233</v>
+        <v>7.9983878000639379</v>
       </c>
       <c r="C5" s="0">
-        <v>22520.736121599999</v>
+        <v>2018076.0186334001</v>
       </c>
       <c r="D5" s="0">
-        <v>22530.736809800001</v>
+        <v>2018084.0189324</v>
       </c>
       <c r="E5" s="0" t="s">
         <v>5</v>
@@ -182,213 +182,241 @@
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>9.9993088999763131</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>2018076.0186073</v>
       </c>
       <c r="D6" s="0">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0"/>
+        <v>2018086.0198535</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>0</v>
+        <v>11.998830100055784</v>
       </c>
       <c r="C7" s="0">
-        <v>0</v>
+        <v>2018076.0186324001</v>
       </c>
       <c r="D7" s="0">
-        <v>0</v>
-      </c>
-      <c r="E7" s="0"/>
+        <v>2018088.0193747</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>0</v>
+        <v>13.999511400004849</v>
       </c>
       <c r="C8" s="0">
-        <v>0</v>
+        <v>2018076.0186307</v>
       </c>
       <c r="D8" s="0">
-        <v>0</v>
-      </c>
-      <c r="E8" s="0"/>
+        <v>2018090.020056</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>0</v>
+        <v>15.998318700119853</v>
       </c>
       <c r="C9" s="0">
-        <v>0</v>
+        <v>2018076.0186332001</v>
       </c>
       <c r="D9" s="0">
-        <v>0</v>
-      </c>
-      <c r="E9" s="0"/>
+        <v>2018092.0188633001</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>0</v>
+        <v>17.998543200083077</v>
       </c>
       <c r="C10" s="0">
-        <v>0</v>
+        <v>2018076.0186333</v>
       </c>
       <c r="D10" s="0">
-        <v>0</v>
-      </c>
-      <c r="E10" s="0"/>
+        <v>2018094.0190878001</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>0</v>
+        <v>19.998396700015292</v>
       </c>
       <c r="C11" s="0">
-        <v>0</v>
+        <v>2018076.0186331</v>
       </c>
       <c r="D11" s="0">
-        <v>0</v>
-      </c>
-      <c r="E11" s="0"/>
+        <v>2018096.0189413</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>0</v>
+        <v>21.998372799949721</v>
       </c>
       <c r="C12" s="0">
-        <v>0</v>
+        <v>2018076.0186329</v>
       </c>
       <c r="D12" s="0">
-        <v>0</v>
-      </c>
-      <c r="E12" s="0"/>
+        <v>2018098.0189173999</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>0</v>
+        <v>23.998295200057328</v>
       </c>
       <c r="C13" s="0">
-        <v>0</v>
+        <v>2018076.0186334001</v>
       </c>
       <c r="D13" s="0">
-        <v>0</v>
-      </c>
-      <c r="E13" s="0"/>
+        <v>2018100.0188398</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>0</v>
+        <v>25.998398100025952</v>
       </c>
       <c r="C14" s="0">
-        <v>0</v>
+        <v>2018076.0186331</v>
       </c>
       <c r="D14" s="0">
-        <v>0</v>
-      </c>
-      <c r="E14" s="0"/>
+        <v>2018102.0189427</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>0</v>
+        <v>27.998278399929404</v>
       </c>
       <c r="C15" s="0">
-        <v>0</v>
+        <v>2018076.0186333</v>
       </c>
       <c r="D15" s="0">
-        <v>0</v>
-      </c>
-      <c r="E15" s="0"/>
+        <v>2018104.0188229999</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>0</v>
+        <v>29.998560100095347</v>
       </c>
       <c r="C16" s="0">
-        <v>0</v>
+        <v>2018076.0186313</v>
       </c>
       <c r="D16" s="0">
-        <v>0</v>
-      </c>
-      <c r="E16" s="0"/>
+        <v>2018106.0191047001</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>0</v>
+        <v>31.998352100141346</v>
       </c>
       <c r="C17" s="0">
-        <v>0</v>
+        <v>2018076.0186328001</v>
       </c>
       <c r="D17" s="0">
-        <v>0</v>
-      </c>
-      <c r="E17" s="0"/>
+        <v>2018108.0188967001</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="0">
-        <v>0</v>
+        <v>33.998800799949095</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>2018076.018499</v>
       </c>
       <c r="D18" s="0">
-        <v>0</v>
-      </c>
-      <c r="E18" s="0"/>
+        <v>2018110.0193453999</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="0">
-        <v>0</v>
+        <v>35.998359200078994</v>
       </c>
       <c r="C19" s="0">
-        <v>0</v>
+        <v>2018076.0186292001</v>
       </c>
       <c r="D19" s="0">
-        <v>0</v>
-      </c>
-      <c r="E19" s="0"/>
+        <v>2018112.0189038001</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="0">

</xml_diff>